<commit_message>
pageobjectframework is committed dated nov14
</commit_message>
<xml_diff>
--- a/PageObjectModelFramework/resources/testdata.xlsx
+++ b/PageObjectModelFramework/resources/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="FindNewCar" sheetId="5" r:id="rId1"/>
@@ -616,14 +616,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>